<commit_message>
Added to Bill of Materials
</commit_message>
<xml_diff>
--- a/Design/Bill of Materials/BOM.xlsx
+++ b/Design/Bill of Materials/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -134,13 +134,32 @@
   </si>
   <si>
     <t>USB A receptacle to USB A plug</t>
+  </si>
+  <si>
+    <t>Nitra Nylon Tubing</t>
+  </si>
+  <si>
+    <t>Flexible Tubing</t>
+  </si>
+  <si>
+    <t>n532BLU100</t>
+  </si>
+  <si>
+    <t>200 ft</t>
+  </si>
+  <si>
+    <t>Bimba Air Cylinder</t>
+  </si>
+  <si>
+    <t>2 IN Bore Diameter Dual Acting Cylinders with position feedback</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -180,9 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -244,7 +265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,7 +300,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,7 +521,8 @@
     <col min="2" max="2" width="80.109375" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -766,7 +788,39 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2831.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>